<commit_message>
improved logic to wait for next run, considering first run and errors
* improve OaiHarvester#waitForNextRun(..), for full details see file
/doc/HarvesterResumptionLogic.xlsx, sheet "waitForNextRun logic".
** do not wait at all if this is the harvesters first run ever (empty
database and there is no previous run that resulted in an error).
Previously, the harvester waited at startup one pollInterval - so
nothing happened after startup.
** when starting up the harvester and a previous OaiRunResult is loaded
from persistence, time to wait is calculated based on timestampLastRun
** consider if an error occurred in the last harvest run and no
OairunResult was written to persistence. An error occurred, iff the OAI
service provider responds with any HTTP status code != 200.
</commit_message>
<xml_diff>
--- a/doc/HarvesterResumptionLogic.xlsx
+++ b/doc/HarvesterResumptionLogic.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="17715" windowHeight="11820"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="17715" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="OaiRunResult processing" sheetId="1" r:id="rId1"/>
+    <sheet name="waitForNextRun logic" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>(last) OaiRunResult loaded from DB</t>
   </si>
@@ -85,15 +85,74 @@
     <t>T</t>
   </si>
   <si>
-    <t>plus Tests, wenn resumptionToken als invalide vom Server gemeldet wird!! - vmtl müssen hierfür auch die nicht erfolgreichen OaiRunResults in der DB gespeichert werden, da sonst immer wieder der invalide resumptionToken verwendet wird!!</t>
+    <t>resumptioToken present</t>
+  </si>
+  <si>
+    <t>lastRunResultedInError</t>
+  </si>
+  <si>
+    <t>timestampLastRun present</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>resulting time to wait till next run</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Impossible. If there is a resumptionToken present, there is always a timestampLastRun present.</t>
+  </si>
+  <si>
+    <t>pollInterval</t>
+  </si>
+  <si>
+    <t>very first run of harvester, start immediately</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If lastRunResultedInError==true, always wait pollInterval. </t>
+  </si>
+  <si>
+    <t>next run is usually at timestampLastRun + pollInterval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The waitTime depends on how much time already passed between the timestampLastRun and the current point in time. We need to wait till timestampLastRun + pollInterval is reached so waitTime is something between 0 and pollInterval. (Here, we need to consider that the harvester may have been shut down after the last successful run has been written to persistence layer.)
+Furthermore, we need to check whether timestampLastRun is in future of now() - if so, this is an error and we wait for a whole pollInterval. </t>
+  </si>
+  <si>
+    <t>minimumWaittimeBetweenTwoRequests</t>
+  </si>
+  <si>
+    <t>We have a resumption token, that means we process an OAI service provider's paginated response. Therefore, we wait a very short time such as 1 second (to avoid beeing blocked by OAI service provider, our requests are no denial-of-service attack)
+It is worth mentioning that we can ignore the potential error that timestampLastRun may be future: 
+* if the resumption token is valid, we get the next page of a paginated response ( and go to case 2 or 3 next time waitForNextRun(..) is called), or
+* if it is invalid, next the run will result in a OAI error "badResumptionToken" and case 2 will be processed next time waitForNextRun(..) is called, or
+* the run will result in an error, so lastRunResultedInError== true next time waitForNextRun(..) is called  (this may always happen)
+=&gt; in any case, we should not end in an infinite loop with case 3, sending requests at a high frequency.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>(4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -115,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -455,11 +514,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -516,6 +685,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,29 +733,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,28 +1145,28 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="26" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="23"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
@@ -926,8 +1176,8 @@
       <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
@@ -957,13 +1207,13 @@
       <c r="F4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="25">
         <v>111</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="26">
         <v>111</v>
       </c>
       <c r="J4" s="19" t="s">
@@ -989,13 +1239,13 @@
       <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="21">
         <v>222</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="20">
         <v>222</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -1021,13 +1271,13 @@
       <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="31" t="s">
+      <c r="G6" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="3" t="s">
@@ -1053,13 +1303,13 @@
       <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="21">
         <v>333</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="20">
         <v>333</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -1082,10 +1332,10 @@
       <c r="F8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="31" t="s">
+      <c r="G8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="22" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1111,10 +1361,10 @@
       <c r="F9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="33" t="s">
+      <c r="G9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -1124,17 +1374,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B12:E12"/>
+  <mergeCells count="5">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="B2:B3"/>
@@ -1148,13 +1395,253 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="93.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="44">
+        <v>1</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="48">
+        <v>0</v>
+      </c>
+      <c r="G3" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="57"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+    </row>
+    <row r="7" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="50">
+        <v>2</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="54"/>
+      <c r="G8" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+    </row>
+    <row r="9" spans="2:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="B9" s="50">
+        <v>3</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="62"/>
+      <c r="G10" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F5:G6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>